<commit_message>
Ajout de la classe cheval
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F4745B-EB72-462E-A471-59B2249E9B37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003C9E4D-892A-4598-B8B8-082F84F79EDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:BA99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <selection activeCell="AB75" sqref="AB75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4141,8 +4141,8 @@
     <row r="73" spans="1:53">
       <c r="A73" s="37"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="18" t="s">
-        <v>16</v>
+      <c r="C73" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="5"/>
@@ -4168,7 +4168,7 @@
       <c r="Y73" s="5"/>
       <c r="Z73" s="5"/>
       <c r="AA73" s="5"/>
-      <c r="AB73" s="18"/>
+      <c r="AB73" s="17"/>
       <c r="AC73" s="5"/>
       <c r="AD73" s="5"/>
       <c r="AE73" s="5"/>
@@ -4207,8 +4207,8 @@
     <row r="75" spans="1:53">
       <c r="A75" s="37"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="13" t="s">
-        <v>20</v>
+      <c r="C75" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="5"/>
@@ -4234,7 +4234,7 @@
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
       <c r="AA75" s="5"/>
-      <c r="AB75" s="5"/>
+      <c r="AB75" s="18"/>
       <c r="AC75" s="5"/>
       <c r="AD75" s="5"/>
       <c r="AE75" s="5"/>

</xml_diff>

<commit_message>
Ajout de la classe Fou.
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003C9E4D-892A-4598-B8B8-082F84F79EDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A5507C-EC58-4699-A030-721610AE7C54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:BA99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB75" sqref="AB75"/>
+      <selection activeCell="X75" sqref="X75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4207,8 +4207,8 @@
     <row r="75" spans="1:53">
       <c r="A75" s="37"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="18" t="s">
-        <v>16</v>
+      <c r="C75" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="5"/>
@@ -4234,7 +4234,7 @@
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
       <c r="AA75" s="5"/>
-      <c r="AB75" s="18"/>
+      <c r="AB75" s="17"/>
       <c r="AC75" s="5"/>
       <c r="AD75" s="5"/>
       <c r="AE75" s="5"/>
@@ -4273,8 +4273,8 @@
     <row r="77" spans="1:53">
       <c r="A77" s="37"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="13" t="s">
-        <v>20</v>
+      <c r="C77" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="5"/>
@@ -4300,7 +4300,7 @@
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
-      <c r="AB77" s="5"/>
+      <c r="AB77" s="18"/>
       <c r="AC77" s="5"/>
       <c r="AD77" s="5"/>
       <c r="AE77" s="5"/>

</xml_diff>

<commit_message>
Classe Dame + classe Pion + Menaces
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A5507C-EC58-4699-A030-721610AE7C54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5188965C-285E-44E6-A06B-E89C537334F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:BA99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X75" sqref="X75"/>
+      <selection activeCell="AC78" sqref="AC78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4273,8 +4273,8 @@
     <row r="77" spans="1:53">
       <c r="A77" s="37"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="18" t="s">
-        <v>16</v>
+      <c r="C77" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="5"/>
@@ -4300,7 +4300,7 @@
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
-      <c r="AB77" s="18"/>
+      <c r="AB77" s="17"/>
       <c r="AC77" s="5"/>
       <c r="AD77" s="5"/>
       <c r="AE77" s="5"/>
@@ -4345,8 +4345,8 @@
     <row r="79" spans="1:53">
       <c r="A79" s="37"/>
       <c r="B79" s="5"/>
-      <c r="C79" s="13" t="s">
-        <v>20</v>
+      <c r="C79" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="5"/>
@@ -4373,9 +4373,9 @@
       <c r="Z79" s="5"/>
       <c r="AA79" s="5"/>
       <c r="AB79" s="5"/>
-      <c r="AC79" s="5"/>
-      <c r="AD79" s="5"/>
-      <c r="AE79" s="5"/>
+      <c r="AC79" s="17"/>
+      <c r="AD79" s="17"/>
+      <c r="AE79" s="18"/>
       <c r="AF79" s="5"/>
       <c r="AG79" s="13"/>
       <c r="AH79" s="12"/>

</xml_diff>

<commit_message>
Amélioration du code et ajout de commentaires
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5188965C-285E-44E6-A06B-E89C537334F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620BE067-D55D-4629-9D15-EB108FB1B535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1457,8 +1457,8 @@
   </sheetPr>
   <dimension ref="A1:BA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC78" sqref="AC78"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC86" sqref="AC86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4630,7 +4630,7 @@
       <c r="AB86" s="43"/>
       <c r="AC86" s="43"/>
       <c r="AD86" s="43"/>
-      <c r="AE86" s="43"/>
+      <c r="AE86" s="46"/>
       <c r="AF86" s="43"/>
       <c r="AG86" s="44"/>
       <c r="AH86" s="45"/>
@@ -4687,7 +4687,7 @@
       <c r="AB87" s="43"/>
       <c r="AC87" s="43"/>
       <c r="AD87" s="43"/>
-      <c r="AE87" s="43"/>
+      <c r="AE87" s="46"/>
       <c r="AF87" s="43"/>
       <c r="AG87" s="44"/>
       <c r="AH87" s="45"/>
@@ -4744,7 +4744,7 @@
       <c r="AB88" s="43"/>
       <c r="AC88" s="43"/>
       <c r="AD88" s="43"/>
-      <c r="AE88" s="43"/>
+      <c r="AE88" s="46"/>
       <c r="AF88" s="43"/>
       <c r="AG88" s="44"/>
       <c r="AH88" s="45"/>

</xml_diff>

<commit_message>
Barre d'évaluation + pions fonctionels
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\chess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gouvernonst\Desktop\Git\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DF5AD8-74B8-4013-AAC3-D098BE7DFD93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562C961F-70E9-45B5-B4A7-97FC76B65667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="110">
   <si>
     <t>Phase</t>
   </si>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:BA99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+      <selection activeCell="AM78" sqref="AM78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4345,8 +4345,8 @@
     <row r="79" spans="1:53">
       <c r="A79" s="37"/>
       <c r="B79" s="5"/>
-      <c r="C79" s="18" t="s">
-        <v>16</v>
+      <c r="C79" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="5"/>
@@ -4377,12 +4377,12 @@
       <c r="AD79" s="17"/>
       <c r="AE79" s="17"/>
       <c r="AF79" s="17"/>
-      <c r="AG79" s="18"/>
-      <c r="AH79" s="12"/>
-      <c r="AI79" s="5"/>
-      <c r="AJ79" s="5"/>
-      <c r="AK79" s="5"/>
-      <c r="AL79" s="5"/>
+      <c r="AG79" s="17"/>
+      <c r="AH79" s="16"/>
+      <c r="AI79" s="17"/>
+      <c r="AJ79" s="17"/>
+      <c r="AK79" s="17"/>
+      <c r="AL79" s="17"/>
       <c r="AM79" s="5"/>
       <c r="AN79" s="5"/>
       <c r="AO79" s="5"/>
@@ -4411,8 +4411,8 @@
     <row r="81" spans="1:53">
       <c r="A81" s="37"/>
       <c r="B81" s="5"/>
-      <c r="C81" s="13" t="s">
-        <v>20</v>
+      <c r="C81" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="D81" s="12"/>
       <c r="E81" s="5"/>
@@ -4449,7 +4449,7 @@
       <c r="AJ81" s="5"/>
       <c r="AK81" s="5"/>
       <c r="AL81" s="5"/>
-      <c r="AM81" s="5"/>
+      <c r="AM81" s="17"/>
       <c r="AN81" s="5"/>
       <c r="AO81" s="5"/>
       <c r="AP81" s="5"/>
@@ -4477,8 +4477,8 @@
     <row r="83" spans="1:53">
       <c r="A83" s="37"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="13" t="s">
-        <v>20</v>
+      <c r="C83" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="5"/>
@@ -4516,7 +4516,7 @@
       <c r="AK83" s="5"/>
       <c r="AL83" s="5"/>
       <c r="AM83" s="5"/>
-      <c r="AN83" s="5"/>
+      <c r="AN83" s="18"/>
       <c r="AO83" s="5"/>
       <c r="AP83" s="5"/>
       <c r="AQ83" s="13"/>

</xml_diff>

<commit_message>
essai pour le mat
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gouvernonst\Desktop\Git\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562C961F-70E9-45B5-B4A7-97FC76B65667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C344C1-0A14-4018-A2FD-71257A23A15D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="110">
   <si>
     <t>Phase</t>
   </si>
@@ -477,7 +477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +505,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -714,6 +720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1457,7 +1464,7 @@
   </sheetPr>
   <dimension ref="A1:BA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AM78" sqref="AM78"/>
     </sheetView>
   </sheetViews>
@@ -4037,7 +4044,7 @@
       <c r="Y69" s="5"/>
       <c r="Z69" s="17"/>
       <c r="AA69" s="17"/>
-      <c r="AB69" s="17"/>
+      <c r="AB69" s="5"/>
       <c r="AC69" s="5"/>
       <c r="AD69" s="5"/>
       <c r="AE69" s="5"/>
@@ -4383,7 +4390,7 @@
       <c r="AJ79" s="17"/>
       <c r="AK79" s="17"/>
       <c r="AL79" s="17"/>
-      <c r="AM79" s="5"/>
+      <c r="AM79" s="17"/>
       <c r="AN79" s="5"/>
       <c r="AO79" s="5"/>
       <c r="AP79" s="5"/>
@@ -4449,8 +4456,8 @@
       <c r="AJ81" s="5"/>
       <c r="AK81" s="5"/>
       <c r="AL81" s="5"/>
-      <c r="AM81" s="17"/>
-      <c r="AN81" s="5"/>
+      <c r="AM81" s="47"/>
+      <c r="AN81" s="17"/>
       <c r="AO81" s="5"/>
       <c r="AP81" s="5"/>
       <c r="AQ81" s="13"/>
@@ -4516,10 +4523,10 @@
       <c r="AK83" s="5"/>
       <c r="AL83" s="5"/>
       <c r="AM83" s="5"/>
-      <c r="AN83" s="18"/>
-      <c r="AO83" s="5"/>
-      <c r="AP83" s="5"/>
-      <c r="AQ83" s="13"/>
+      <c r="AN83" s="47"/>
+      <c r="AO83" s="17"/>
+      <c r="AP83" s="17"/>
+      <c r="AQ83" s="17"/>
       <c r="AR83" s="12"/>
       <c r="AS83" s="5"/>
       <c r="AT83" s="5"/>
@@ -4642,7 +4649,7 @@
       <c r="AN86" s="43"/>
       <c r="AO86" s="43"/>
       <c r="AP86" s="43"/>
-      <c r="AQ86" s="44"/>
+      <c r="AQ86" s="18"/>
       <c r="AR86" s="45"/>
       <c r="AS86" s="43"/>
       <c r="AT86" s="43"/>
@@ -4699,7 +4706,7 @@
       <c r="AN87" s="43"/>
       <c r="AO87" s="43"/>
       <c r="AP87" s="43"/>
-      <c r="AQ87" s="44"/>
+      <c r="AQ87" s="18"/>
       <c r="AR87" s="45"/>
       <c r="AS87" s="43"/>
       <c r="AT87" s="43"/>
@@ -4756,7 +4763,7 @@
       <c r="AN88" s="43"/>
       <c r="AO88" s="43"/>
       <c r="AP88" s="43"/>
-      <c r="AQ88" s="44"/>
+      <c r="AQ88" s="18"/>
       <c r="AR88" s="45"/>
       <c r="AS88" s="43"/>
       <c r="AT88" s="43"/>

</xml_diff>